<commit_message>
Formatting changes to manuscript figures
</commit_message>
<xml_diff>
--- a/Computational_Data/Overview_Energies/CASSCF_Energies.xlsx
+++ b/Computational_Data/Overview_Energies/CASSCF_Energies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jacob/Documents/Water_Splitting/Two_Photon_Water_Splitting/Computational_Data/Overview_Energies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E086A695-6934-774C-8758-EEC49A97071E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593E9E6E-5896-BE41-8A60-91EFA9042C77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19580" windowHeight="13320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19580" windowHeight="13320" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAS1311 Pi VDZ" sheetId="1" r:id="rId1"/>
@@ -117,12 +117,6 @@
     <t>D$_{1}$/D$_{0}$;MECI</t>
   </si>
   <si>
-    <t>$\bf{C_{mono}}$</t>
-  </si>
-  <si>
-    <t>FC;$\bf{B_{mono}}$</t>
-  </si>
-  <si>
     <t>Image</t>
   </si>
   <si>
@@ -196,6 +190,12 @@
   </si>
   <si>
     <t>VDZ kJ/mol Root 5</t>
+  </si>
+  <si>
+    <t>[$\bf{C-Mono}$]</t>
+  </si>
+  <si>
+    <t>[$\bf{B-Mono}$];FC</t>
   </si>
 </sst>
 </file>
@@ -635,7 +635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -745,7 +745,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -762,7 +762,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B8">
         <v>4.3745289151251603</v>
@@ -779,7 +779,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B9">
         <v>248.01854257975197</v>
@@ -796,7 +796,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B10">
         <v>272.76117343991154</v>
@@ -813,7 +813,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B11">
         <v>410.92289918891049</v>
@@ -1042,7 +1042,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1060,7 +1060,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B8">
         <v>21.063675593272041</v>
@@ -1078,7 +1078,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9">
         <v>251.11348168269438</v>
@@ -1096,7 +1096,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10">
         <v>265.60135686212311</v>
@@ -1114,7 +1114,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11">
         <v>290.57939002968834</v>
@@ -1152,8 +1152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1169,22 +1169,22 @@
         <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" t="s">
-        <v>35</v>
-      </c>
       <c r="H1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1192,13 +1192,13 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
         <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
       </c>
       <c r="E2">
         <v>8.5000000000000006E-2</v>
@@ -1210,7 +1210,7 @@
         <v>-1.4999999999999999E-2</v>
       </c>
       <c r="H2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I2">
         <v>-0.7</v>
@@ -1221,13 +1221,13 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E3">
         <v>0.09</v>
@@ -1239,7 +1239,7 @@
         <v>-0.05</v>
       </c>
       <c r="H3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1250,13 +1250,13 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E4">
         <v>0.1</v>
@@ -1268,7 +1268,7 @@
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="H4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -1279,13 +1279,13 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E5">
         <v>0.09</v>
@@ -1297,7 +1297,7 @@
         <v>-0.17</v>
       </c>
       <c r="H5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I5">
         <v>-1.1499999999999999</v>

</xml_diff>